<commit_message>
openai integration, table column classification for excel output
</commit_message>
<xml_diff>
--- a/resources/xlsx_templates/archive.xlsx
+++ b/resources/xlsx_templates/archive.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbrandt/code/birddog/resources/xlsx_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15CB2E9-21B3-3E41-8966-F22E5E7F89C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7502FB38-3159-6F47-BF01-41A529A13004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1980" yWindow="7620" windowWidth="29180" windowHeight="9640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -134,15 +134,6 @@
     <t>{edit:changed}</t>
   </si>
   <si>
-    <t>{child[0]:linked}</t>
-  </si>
-  <si>
-    <t>{child[1]:linked}</t>
-  </si>
-  <si>
-    <t>{child[2]}</t>
-  </si>
-  <si>
     <t>='{child:sheetname}'!E5</t>
   </si>
   <si>
@@ -177,6 +168,15 @@
   </si>
   <si>
     <t>{edit:unlinked}</t>
+  </si>
+  <si>
+    <t>{child[ID]:linked}</t>
+  </si>
+  <si>
+    <t>{child[DESCRIPTION]:linked}</t>
+  </si>
+  <si>
+    <t>{child[DATE]}</t>
   </si>
 </sst>
 </file>
@@ -919,9 +919,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P2" sqref="P2:P3"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -972,7 +972,7 @@
         <v>31</v>
       </c>
       <c r="P2" s="63" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -1002,7 +1002,7 @@
         <v>32</v>
       </c>
       <c r="P3" s="64" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1">
@@ -1133,46 +1133,46 @@
     </row>
     <row r="8" spans="1:16" ht="15" customHeight="1">
       <c r="A8" s="49" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="C8" s="51" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="D8" s="52" t="s">
         <v>27</v>
       </c>
       <c r="E8" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="53" t="s">
+      <c r="I8" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="53" t="s">
+      <c r="J8" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="53" t="s">
+      <c r="K8" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="I8" s="53" t="s">
+      <c r="L8" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="J8" s="53" t="s">
+      <c r="M8" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="K8" s="53" t="s">
+      <c r="N8" s="53" t="s">
         <v>42</v>
-      </c>
-      <c r="L8" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="M8" s="53" t="s">
-        <v>44</v>
-      </c>
-      <c r="N8" s="53" t="s">
-        <v>45</v>
       </c>
       <c r="O8" s="54" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
date formatting for export
</commit_message>
<xml_diff>
--- a/resources/xlsx_templates/archive.xlsx
+++ b/resources/xlsx_templates/archive.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbrandt/code/birddog/resources/xlsx_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7502FB38-3159-6F47-BF01-41A529A13004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC444E8-C39E-CD40-B594-437123A56A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="7620" windowWidth="29180" windowHeight="9640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1980" yWindow="7620" windowWidth="33500" windowHeight="10180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="{id}" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
   <si>
     <t>accessed:</t>
   </si>
@@ -110,9 +110,6 @@
     <t>{description}</t>
   </si>
   <si>
-    <t>{lastmod}</t>
-  </si>
-  <si>
     <t>{url:linked}</t>
   </si>
   <si>
@@ -177,6 +174,15 @@
   </si>
   <si>
     <t>{child[DATE]}</t>
+  </si>
+  <si>
+    <t>{lastmod:date}</t>
+  </si>
+  <si>
+    <t>ref. version</t>
+  </si>
+  <si>
+    <t>{refmod:date}</t>
   </si>
 </sst>
 </file>
@@ -342,15 +348,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF7030A0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1" tint="0.499984740745262"/>
       <name val="Calibri"/>
@@ -920,8 +926,8 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P3" sqref="P2:P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -969,10 +975,10 @@
       <c r="M2" s="10"/>
       <c r="N2" s="9"/>
       <c r="O2" s="60" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P2" s="63" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -981,15 +987,15 @@
       <c r="C3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>25</v>
+      <c r="D3" s="24" t="s">
+        <v>47</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3" s="16" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H3" s="14"/>
       <c r="I3" s="18"/>
@@ -999,10 +1005,10 @@
       <c r="M3" s="20"/>
       <c r="N3" s="20"/>
       <c r="O3" s="61" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P3" s="64" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1">
@@ -1012,8 +1018,12 @@
       <c r="B4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24"/>
+      <c r="C4" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>49</v>
+      </c>
       <c r="E4" s="23"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
@@ -1034,34 +1044,34 @@
         <v>4</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" s="30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G5" s="30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I5" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J5" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K5" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L5" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M5" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N5" s="33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O5" s="23"/>
     </row>
@@ -1133,49 +1143,49 @@
     </row>
     <row r="8" spans="1:16" ht="15" customHeight="1">
       <c r="A8" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="C8" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="51" t="s">
-        <v>47</v>
-      </c>
       <c r="D8" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="53" t="s">
+      <c r="G8" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="53" t="s">
+      <c r="H8" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="53" t="s">
+      <c r="I8" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="I8" s="53" t="s">
+      <c r="J8" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="J8" s="53" t="s">
+      <c r="K8" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="K8" s="53" t="s">
+      <c r="L8" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="L8" s="53" t="s">
+      <c r="M8" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="M8" s="53" t="s">
+      <c r="N8" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="53" t="s">
-        <v>42</v>
-      </c>
       <c r="O8" s="54" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" customHeight="1">
@@ -1197,7 +1207,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="57" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="58" t="s">
         <v>21</v>
@@ -1215,7 +1225,7 @@
         <v>22</v>
       </c>
       <c r="M10" s="62" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N10" s="58"/>
       <c r="O10" s="58"/>

</xml_diff>

<commit_message>
lower wiki page requests with throttling and HistoryLRU cache; logging endpoint
</commit_message>
<xml_diff>
--- a/resources/xlsx_templates/archive.xlsx
+++ b/resources/xlsx_templates/archive.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbrandt/code/birddog/resources/xlsx_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC444E8-C39E-CD40-B594-437123A56A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D97B65-2FCF-FA43-890D-6EA5A6E50E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1980" yWindow="7620" windowWidth="33500" windowHeight="10180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
   <si>
     <t>accessed:</t>
   </si>
@@ -129,36 +129,6 @@
   </si>
   <si>
     <t>{edit:changed}</t>
-  </si>
-  <si>
-    <t>='{child:sheetname}'!E5</t>
-  </si>
-  <si>
-    <t>='{child:sheetname}'!F5</t>
-  </si>
-  <si>
-    <t>='{child:sheetname}'!G5</t>
-  </si>
-  <si>
-    <t>='{child:sheetname}'!H5</t>
-  </si>
-  <si>
-    <t>='{child:sheetname}'!I5</t>
-  </si>
-  <si>
-    <t>='{child:sheetname}'!J5</t>
-  </si>
-  <si>
-    <t>='{child:sheetname}'!K5</t>
-  </si>
-  <si>
-    <t>='{child:sheetname}'!L5</t>
-  </si>
-  <si>
-    <t>='{child:sheetname}'!M5</t>
-  </si>
-  <si>
-    <t>='{child:sheetname}'!N5</t>
   </si>
   <si>
     <t>{edit:linked}</t>
@@ -450,7 +420,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -512,12 +482,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -669,18 +667,6 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -707,6 +693,15 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -927,7 +922,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P3" sqref="P2:P3"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -974,11 +969,11 @@
       <c r="L2" s="10"/>
       <c r="M2" s="10"/>
       <c r="N2" s="9"/>
-      <c r="O2" s="60" t="s">
+      <c r="O2" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="63" t="s">
-        <v>42</v>
+      <c r="P2" s="59" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -988,7 +983,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3" s="16" t="s">
@@ -1004,11 +999,11 @@
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
       <c r="N3" s="20"/>
-      <c r="O3" s="61" t="s">
+      <c r="O3" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="P3" s="64" t="s">
-        <v>43</v>
+      <c r="P3" s="60" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1">
@@ -1019,10 +1014,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E4" s="23"/>
       <c r="F4" s="14"/>
@@ -1143,53 +1138,53 @@
     </row>
     <row r="8" spans="1:16" ht="15" customHeight="1">
       <c r="A8" s="49" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="51" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="53" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="53" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="J8" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="K8" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="L8" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="M8" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="N8" s="53" t="s">
-        <v>41</v>
-      </c>
-      <c r="O8" s="54" t="s">
+      <c r="E8" s="63" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="63" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="63" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="63" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="63" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="63" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="63" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" s="63" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="63" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" s="63" t="s">
+        <v>26</v>
+      </c>
+      <c r="O8" s="63" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A9" s="55"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="27"/>
       <c r="C9" s="28"/>
       <c r="D9" s="28"/>
@@ -1198,37 +1193,37 @@
       <c r="G9" s="28"/>
       <c r="H9" s="28"/>
       <c r="I9" s="28"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="56"/>
-      <c r="L9" s="56"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
       <c r="M9" s="42"/>
       <c r="N9" s="42"/>
       <c r="O9" s="42"/>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="58"/>
-      <c r="I10" s="58"/>
-      <c r="J10" s="58"/>
-      <c r="K10" s="58"/>
-      <c r="L10" s="59" t="s">
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="M10" s="62" t="s">
+      <c r="M10" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="N10" s="58"/>
-      <c r="O10" s="58"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="54"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
use google cloud translate; template tweaks
</commit_message>
<xml_diff>
--- a/resources/xlsx_templates/archive.xlsx
+++ b/resources/xlsx_templates/archive.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbrandt/code/birddog/resources/xlsx_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0767AE0A-41E7-F748-8627-7916E4C92892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEAE3FB1-53C9-924E-9BDB-F3404BADF46C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10880" yWindow="9920" windowWidth="51660" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
   <si>
     <t>source:</t>
   </si>
@@ -135,9 +135,6 @@
   </si>
   <si>
     <t>{lastmod:date}</t>
-  </si>
-  <si>
-    <t>{refmod:date}</t>
   </si>
   <si>
     <t>wiki</t>
@@ -904,7 +901,7 @@
   <dimension ref="A1:AB21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15"/>
@@ -916,11 +913,11 @@
   <sheetData>
     <row r="1" spans="1:28" ht="28">
       <c r="A1" s="42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="43"/>
       <c r="C1" s="44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D1" s="45"/>
       <c r="E1" s="46"/>
@@ -930,16 +927,14 @@
       <c r="I1" s="42"/>
       <c r="J1" s="46"/>
       <c r="K1" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="50"/>
+      <c r="M1" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="N1" s="51" t="s">
         <v>33</v>
-      </c>
-      <c r="M1" s="49" t="s">
-        <v>37</v>
-      </c>
-      <c r="N1" s="51" t="s">
-        <v>34</v>
       </c>
       <c r="O1" s="38" t="s">
         <v>26</v>
@@ -959,7 +954,7 @@
     </row>
     <row r="2" spans="1:28" ht="19">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
@@ -997,7 +992,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="8"/>

</xml_diff>